<commit_message>
Added repo content to read me file and added print statement to deeplearning_main code
</commit_message>
<xml_diff>
--- a/Projects/SentimentAnalysis/Data/Process/Summary.xlsx
+++ b/Projects/SentimentAnalysis/Data/Process/Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravip\Documents\Data-Science\Projects\SentimentAnalysis\Data\Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A5C80F-C4D5-46EA-AB45-F629EA9D3213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E600B56-8744-4FB2-A802-591B0991B5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -157,18 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -267,6 +262,62 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -2938,7 +2989,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{08A4A332-A92F-456C-94F9-28947F80947A}" name="PivotTable18" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{08A4A332-A92F-456C-94F9-28947F80947A}" name="PivotTable18" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A24:D32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -3081,7 +3132,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31BDA639-D35B-4860-B480-3848121B21F4}" name="PivotTable17" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31BDA639-D35B-4860-B480-3848121B21F4}" name="PivotTable17" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A4:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -3164,7 +3215,7 @@
   <dataFields count="1">
     <dataField name="Sum of accuracy" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3182,6 +3233,18 @@
           </reference>
           <reference field="8" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -3484,10 +3547,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3500,31 +3564,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3760,56 +3824,56 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
-        <v>0.59099999999999997</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>0.59245464546454651</v>
+        <v>0.76180682898532037</v>
       </c>
       <c r="E10" s="1">
-        <v>0.59099999999999997</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="F10" s="1">
-        <v>0.59135831393456983</v>
+        <v>0.76179329644879046</v>
       </c>
       <c r="G10" s="1">
-        <v>21.181067228317261</v>
+        <v>8.59708571434021</v>
       </c>
       <c r="H10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>0.59599999999999997</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="D11" s="1">
-        <v>0.59531684174855992</v>
+        <v>0.73791233766233766</v>
       </c>
       <c r="E11" s="1">
-        <v>0.59599999999999997</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="F11" s="1">
-        <v>0.59550588197428356</v>
+        <v>0.73728682326847461</v>
       </c>
       <c r="G11" s="1">
-        <v>22.867355346679691</v>
+        <v>9.7216942310333252</v>
       </c>
       <c r="H11" s="1" t="b">
         <v>0</v>
@@ -3820,25 +3884,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="D12" s="1">
-        <v>0.54854312354312351</v>
+        <v>0.73023276562206185</v>
       </c>
       <c r="E12" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="F12" s="1">
-        <v>0.51141719216727521</v>
+        <v>0.72923093715296239</v>
       </c>
       <c r="G12" s="1">
-        <v>18.88773083686829</v>
+        <v>4.0309455394744873</v>
       </c>
       <c r="H12" s="1" t="b">
         <v>0</v>
@@ -3847,114 +3911,114 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
-        <v>0.70099999999999996</v>
+        <v>0.72</v>
       </c>
       <c r="D13" s="1">
-        <v>0.70149267542331128</v>
+        <v>0.71967676767676769</v>
       </c>
       <c r="E13" s="1">
-        <v>0.70099999999999996</v>
+        <v>0.72</v>
       </c>
       <c r="F13" s="1">
-        <v>0.70116154887885818</v>
+        <v>0.71954911433172308</v>
       </c>
       <c r="G13" s="1">
-        <v>39.111194610595703</v>
+        <v>21.597750663757321</v>
       </c>
       <c r="H13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
-        <v>0.50800000000000001</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="D14" s="1">
-        <v>0.5238658088235294</v>
+        <v>0.71782745753988686</v>
       </c>
       <c r="E14" s="1">
-        <v>0.50800000000000001</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="F14" s="1">
-        <v>0.49214526854219948</v>
+        <v>0.71788783942855072</v>
       </c>
       <c r="G14" s="1">
-        <v>22.277244806289669</v>
+        <v>7.3510808944702148</v>
       </c>
       <c r="H14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1">
-        <v>0.67900000000000005</v>
+        <v>0.71</v>
       </c>
       <c r="D15" s="1">
-        <v>0.67986234694653591</v>
+        <v>0.70965875947890344</v>
       </c>
       <c r="E15" s="1">
-        <v>0.67900000000000005</v>
+        <v>0.71</v>
       </c>
       <c r="F15" s="1">
-        <v>0.67923508567341018</v>
+        <v>0.70934672840327062</v>
       </c>
       <c r="G15" s="1">
-        <v>35.40446400642395</v>
+        <v>23.60035943984985</v>
       </c>
       <c r="H15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>0.68100000000000005</v>
+        <v>0.71</v>
       </c>
       <c r="D16" s="1">
-        <v>0.68440240918501782</v>
+        <v>0.71273709483793524</v>
       </c>
       <c r="E16" s="1">
-        <v>0.68100000000000005</v>
+        <v>0.71</v>
       </c>
       <c r="F16" s="1">
-        <v>0.6811949419451887</v>
+        <v>0.71023209283713484</v>
       </c>
       <c r="G16" s="1">
-        <v>16.660394430160519</v>
+        <v>5.5891282558441162</v>
       </c>
       <c r="H16" s="1" t="b">
         <v>0</v>
@@ -3965,25 +4029,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>0.625</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="D17" s="1">
-        <v>0.62398619306064684</v>
+        <v>0.70149267542331128</v>
       </c>
       <c r="E17" s="1">
-        <v>0.625</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="F17" s="1">
-        <v>0.6235377939181922</v>
+        <v>0.70116154887885818</v>
       </c>
       <c r="G17" s="1">
-        <v>19.22005724906921</v>
+        <v>39.111194610595703</v>
       </c>
       <c r="H17" s="1" t="b">
         <v>0</v>
@@ -4000,83 +4064,83 @@
         <v>14</v>
       </c>
       <c r="C18" s="1">
-        <v>0.72</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="D18" s="1">
-        <v>0.71967676767676769</v>
+        <v>0.68440240918501782</v>
       </c>
       <c r="E18" s="1">
-        <v>0.72</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="F18" s="1">
-        <v>0.71954911433172308</v>
+        <v>0.6811949419451887</v>
       </c>
       <c r="G18" s="1">
-        <v>21.597750663757321</v>
+        <v>16.660394430160519</v>
       </c>
       <c r="H18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1">
-        <v>0.59</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="D19" s="1">
-        <v>0.59544707455808177</v>
+        <v>0.6808912020762441</v>
       </c>
       <c r="E19" s="1">
-        <v>0.59</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="F19" s="1">
-        <v>0.58964570898209334</v>
+        <v>0.6809394687514746</v>
       </c>
       <c r="G19" s="1">
-        <v>17.604587554931641</v>
+        <v>11.840480327606199</v>
       </c>
       <c r="H19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1">
-        <v>0.60899999999999999</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="D20" s="1">
-        <v>0.61017797766476334</v>
+        <v>0.67986234694653591</v>
       </c>
       <c r="E20" s="1">
-        <v>0.60899999999999999</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="F20" s="1">
-        <v>0.60932071681026834</v>
+        <v>0.67923508567341018</v>
       </c>
       <c r="G20" s="1">
-        <v>22.450376510620121</v>
+        <v>35.40446400642395</v>
       </c>
       <c r="H20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -4108,7 +4172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -4139,25 +4203,25 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1">
-        <v>0.60499999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="D23" s="1">
-        <v>0.60869980879541119</v>
+        <v>0.62398619306064684</v>
       </c>
       <c r="E23" s="1">
-        <v>0.60499999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="F23" s="1">
-        <v>0.60514655218105695</v>
+        <v>0.6235377939181922</v>
       </c>
       <c r="G23" s="1">
-        <v>17.354134082794189</v>
+        <v>19.22005724906921</v>
       </c>
       <c r="H23" s="1" t="b">
         <v>0</v>
@@ -4168,25 +4232,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1">
-        <v>0.53500000000000003</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="D24" s="1">
-        <v>0.56122149899128315</v>
+        <v>0.61791719202180673</v>
       </c>
       <c r="E24" s="1">
-        <v>0.53500000000000003</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="F24" s="1">
-        <v>0.39628951352827552</v>
+        <v>0.61728049162902199</v>
       </c>
       <c r="G24" s="1">
-        <v>31.61168456077576</v>
+        <v>4.6047906875610352</v>
       </c>
       <c r="H24" s="1" t="b">
         <v>0</v>
@@ -4195,27 +4259,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
-        <v>0.71</v>
+        <v>0.61</v>
       </c>
       <c r="D25" s="1">
-        <v>0.70965875947890344</v>
+        <v>0.61098552766393432</v>
       </c>
       <c r="E25" s="1">
-        <v>0.71</v>
+        <v>0.61</v>
       </c>
       <c r="F25" s="1">
-        <v>0.70934672840327062</v>
+        <v>0.61029536101683357</v>
       </c>
       <c r="G25" s="1">
-        <v>23.60035943984985</v>
+        <v>7.942906379699707</v>
       </c>
       <c r="H25" s="1" t="b">
         <v>0</v>
@@ -4224,56 +4288,56 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1">
-        <v>0.61699999999999999</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="D26" s="1">
-        <v>0.61791719202180673</v>
+        <v>0.61017797766476334</v>
       </c>
       <c r="E26" s="1">
-        <v>0.61699999999999999</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="F26" s="1">
-        <v>0.61728049162902199</v>
+        <v>0.60932071681026834</v>
       </c>
       <c r="G26" s="1">
-        <v>4.6047906875610352</v>
+        <v>22.450376510620121</v>
       </c>
       <c r="H26" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1">
-        <v>0.61</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="D27" s="1">
-        <v>0.61098552766393432</v>
+        <v>0.60751600102406556</v>
       </c>
       <c r="E27" s="1">
-        <v>0.61</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="F27" s="1">
-        <v>0.61029536101683357</v>
+        <v>0.60634869909615519</v>
       </c>
       <c r="G27" s="1">
-        <v>7.942906379699707</v>
+        <v>7.2929322719573966</v>
       </c>
       <c r="H27" s="1" t="b">
         <v>0</v>
@@ -4284,25 +4348,25 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1">
-        <v>0.505</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="D28" s="1">
-        <v>0.50960479887085386</v>
+        <v>0.60869980879541119</v>
       </c>
       <c r="E28" s="1">
-        <v>0.505</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="F28" s="1">
-        <v>0.5044429996749269</v>
+        <v>0.60514655218105695</v>
       </c>
       <c r="G28" s="1">
-        <v>4.5924437046051034</v>
+        <v>17.354134082794189</v>
       </c>
       <c r="H28" s="1" t="b">
         <v>0</v>
@@ -4311,27 +4375,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1">
-        <v>0.52400000000000002</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="D29" s="1">
-        <v>0.537320355392369</v>
+        <v>0.59531684174855992</v>
       </c>
       <c r="E29" s="1">
-        <v>0.52400000000000002</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="F29" s="1">
-        <v>0.51526153049165468</v>
+        <v>0.59550588197428356</v>
       </c>
       <c r="G29" s="1">
-        <v>8.5970227718353271</v>
+        <v>22.867355346679691</v>
       </c>
       <c r="H29" s="1" t="b">
         <v>0</v>
@@ -4342,25 +4406,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1">
-        <v>0.72899999999999998</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="D30" s="1">
-        <v>0.73023276562206185</v>
+        <v>0.59245464546454651</v>
       </c>
       <c r="E30" s="1">
-        <v>0.72899999999999998</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="F30" s="1">
-        <v>0.72923093715296239</v>
+        <v>0.59135831393456983</v>
       </c>
       <c r="G30" s="1">
-        <v>4.0309455394744873</v>
+        <v>21.181067228317261</v>
       </c>
       <c r="H30" s="1" t="b">
         <v>0</v>
@@ -4371,31 +4435,31 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1">
-        <v>0.76200000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="D31" s="1">
-        <v>0.76180682898532037</v>
+        <v>0.59544707455808177</v>
       </c>
       <c r="E31" s="1">
-        <v>0.76200000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="F31" s="1">
-        <v>0.76179329644879046</v>
+        <v>0.58964570898209334</v>
       </c>
       <c r="G31" s="1">
-        <v>8.59708571434021</v>
+        <v>17.604587554931641</v>
       </c>
       <c r="H31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -4429,54 +4493,54 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
-        <v>0.60599999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D33" s="1">
-        <v>0.60751600102406556</v>
+        <v>0.54854312354312351</v>
       </c>
       <c r="E33" s="1">
-        <v>0.60599999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F33" s="1">
-        <v>0.60634869909615519</v>
+        <v>0.51141719216727521</v>
       </c>
       <c r="G33" s="1">
-        <v>7.2929322719573966</v>
+        <v>18.88773083686829</v>
       </c>
       <c r="H33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1">
-        <v>0.71799999999999997</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="D34" s="1">
-        <v>0.71782745753988686</v>
+        <v>0.56122149899128315</v>
       </c>
       <c r="E34" s="1">
-        <v>0.71799999999999997</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="F34" s="1">
-        <v>0.71788783942855072</v>
+        <v>0.39628951352827552</v>
       </c>
       <c r="G34" s="1">
-        <v>7.3510808944702148</v>
+        <v>31.61168456077576</v>
       </c>
       <c r="H34" s="1" t="b">
         <v>0</v>
@@ -4485,27 +4549,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1">
-        <v>0.68100000000000005</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="D35" s="1">
-        <v>0.6808912020762441</v>
+        <v>0.537320355392369</v>
       </c>
       <c r="E35" s="1">
-        <v>0.68100000000000005</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="F35" s="1">
-        <v>0.6809394687514746</v>
+        <v>0.51526153049165468</v>
       </c>
       <c r="G35" s="1">
-        <v>11.840480327606199</v>
+        <v>8.5970227718353271</v>
       </c>
       <c r="H35" s="1" t="b">
         <v>0</v>
@@ -4514,33 +4578,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>0.71</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="D36" s="1">
-        <v>0.71273709483793524</v>
+        <v>0.5238658088235294</v>
       </c>
       <c r="E36" s="1">
-        <v>0.71</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="F36" s="1">
-        <v>0.71023209283713484</v>
+        <v>0.49214526854219948</v>
       </c>
       <c r="G36" s="1">
-        <v>5.5891282558441162</v>
+        <v>22.277244806289669</v>
       </c>
       <c r="H36" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -4548,33 +4612,40 @@
         <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="1">
-        <v>0.73799999999999999</v>
+        <v>0.505</v>
       </c>
       <c r="D37" s="1">
-        <v>0.73791233766233766</v>
+        <v>0.50960479887085386</v>
       </c>
       <c r="E37" s="1">
-        <v>0.73799999999999999</v>
+        <v>0.505</v>
       </c>
       <c r="F37" s="1">
-        <v>0.73728682326847461</v>
+        <v>0.5044429996749269</v>
       </c>
       <c r="G37" s="1">
-        <v>9.7216942310333252</v>
+        <v>4.5924437046051034</v>
       </c>
       <c r="H37" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
-    <sortCondition descending="1" ref="C2:C25"/>
+  <autoFilter ref="A1:I37" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="cleaned"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I37">
+    <sortCondition descending="1" ref="C2:C37"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4597,266 +4668,258 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>0.61699999999999999</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>0.61</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>1.2269999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>0.505</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>0.52400000000000002</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>1.0289999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>0.72899999999999998</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <v>0.76200000000000001</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>1.4910000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>0.57799999999999996</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>0.60599999999999998</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>1.1839999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>0.71799999999999997</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <v>0.68100000000000005</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>1.399</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11">
         <v>0.71</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11">
         <v>0.73799999999999999</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11">
         <v>1.448</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12">
         <v>3.8569999999999998</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12">
         <v>3.9209999999999998</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12">
         <v>7.7780000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26">
         <v>0.59099999999999997</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26">
         <v>0.59599999999999997</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26">
         <v>1.1869999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27">
         <v>0.50800000000000001</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27">
         <v>1.0580000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28">
         <v>0.68100000000000005</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28">
         <v>0.72</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28">
         <v>1.401</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29">
         <v>0.59</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29">
         <v>0.60899999999999999</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29">
         <v>1.1989999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30">
         <v>0.66400000000000003</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30">
         <v>0.64700000000000002</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30">
         <v>1.3109999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31">
         <v>0.60499999999999998</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31">
         <v>0.71</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31">
         <v>1.3149999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32">
         <v>3.681</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32">
         <v>3.79</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32">
         <v>7.4710000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did data cleaning by checking oov from word2vec
</commit_message>
<xml_diff>
--- a/Projects/SentimentAnalysis/Data/Process/Summary.xlsx
+++ b/Projects/SentimentAnalysis/Data/Process/Summary.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravip\Documents\Data-Science\Projects\SentimentAnalysis\Data\Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E600B56-8744-4FB2-A802-591B0991B5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE955E5-A1BF-4214-AA23-A9109D558497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Raw vs cleaned text" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$H$37</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="26">
   <si>
     <t>vectorizer</t>
   </si>
@@ -45,9 +46,6 @@
   </si>
   <si>
     <t>f1</t>
-  </si>
-  <si>
-    <t>time_taken</t>
   </si>
   <si>
     <t>count</t>
@@ -103,6 +101,12 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>cleaned_review</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,11 +157,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -167,6 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2533,7 +2551,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="ravipati venkatesh" refreshedDate="45471.425332407409" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="36" xr:uid="{06454BC2-BBDC-4053-90EE-BD26F4728284}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I37" sheet="Summary"/>
+    <worksheetSource ref="A1:H37" sheet="Summary"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="vectorizer" numFmtId="0">
@@ -2989,7 +3007,138 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{08A4A332-A92F-456C-94F9-28947F80947A}" name="PivotTable18" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31BDA639-D35B-4860-B480-3848121B21F4}" name="PivotTable17" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A4:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="9">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="8"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of accuracy" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{08A4A332-A92F-456C-94F9-28947F80947A}" name="PivotTable18" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A24:D32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -3114,137 +3263,6 @@
           </reference>
           <reference field="8" count="1" selected="0">
             <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31BDA639-D35B-4860-B480-3848121B21F4}" name="PivotTable17" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A4:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="9">
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="4"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="8"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="0" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of accuracy" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -3548,22 +3566,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3583,21 +3601,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>0.85199999999999998</v>
@@ -3611,22 +3626,19 @@
       <c r="F2" s="1">
         <v>0.85212378791335008</v>
       </c>
-      <c r="G2" s="1">
-        <v>1116.9175643920901</v>
-      </c>
-      <c r="H2" s="1" t="b">
+      <c r="G2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>0.85099999999999998</v>
@@ -3640,22 +3652,19 @@
       <c r="F3" s="1">
         <v>0.8511340637476118</v>
       </c>
-      <c r="G3" s="1">
-        <v>27.574214696884159</v>
-      </c>
-      <c r="H3" s="1" t="b">
+      <c r="G3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>0.84499999999999997</v>
@@ -3669,22 +3678,19 @@
       <c r="F4" s="1">
         <v>0.84513208582549515</v>
       </c>
-      <c r="G4" s="1">
-        <v>23.932280540466309</v>
-      </c>
-      <c r="H4" s="1" t="b">
+      <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>0.82599999999999996</v>
@@ -3698,22 +3704,19 @@
       <c r="F5" s="1">
         <v>0.82497375072914636</v>
       </c>
-      <c r="G5" s="1">
-        <v>24.180620908737179</v>
-      </c>
-      <c r="H5" s="1" t="b">
+      <c r="G5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>0.82499999999999996</v>
@@ -3727,22 +3730,19 @@
       <c r="F6" s="1">
         <v>0.82496679320221955</v>
       </c>
-      <c r="G6" s="1">
-        <v>74.01381516456604</v>
-      </c>
-      <c r="H6" s="1" t="b">
+      <c r="G6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>0.82499999999999996</v>
@@ -3756,22 +3756,19 @@
       <c r="F7" s="1">
         <v>0.82506510788805754</v>
       </c>
-      <c r="G7" s="1">
-        <v>72.700642585754395</v>
-      </c>
-      <c r="H7" s="1" t="b">
+      <c r="G7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
         <v>0.82199999999999995</v>
@@ -3785,22 +3782,19 @@
       <c r="F8" s="1">
         <v>0.82207405273937539</v>
       </c>
-      <c r="G8" s="1">
-        <v>985.83105111122131</v>
-      </c>
-      <c r="H8" s="1" t="b">
+      <c r="G8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <v>0.81200000000000006</v>
@@ -3814,51 +3808,45 @@
       <c r="F9" s="1">
         <v>0.81144180342418237</v>
       </c>
-      <c r="G9" s="1">
-        <v>19.05355596542358</v>
-      </c>
-      <c r="H9" s="1" t="b">
+      <c r="G9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.76180682898532037</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.76179329644879046</v>
+      </c>
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.76180682898532037</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.76179329644879046</v>
-      </c>
-      <c r="G10" s="1">
-        <v>8.59708571434021</v>
-      </c>
-      <c r="H10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>0.73799999999999999</v>
@@ -3872,22 +3860,19 @@
       <c r="F11" s="1">
         <v>0.73728682326847461</v>
       </c>
-      <c r="G11" s="1">
-        <v>9.7216942310333252</v>
-      </c>
-      <c r="H11" s="1" t="b">
+      <c r="G11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>0.72899999999999998</v>
@@ -3901,51 +3886,45 @@
       <c r="F12" s="1">
         <v>0.72923093715296239</v>
       </c>
-      <c r="G12" s="1">
-        <v>4.0309455394744873</v>
-      </c>
-      <c r="H12" s="1" t="b">
+      <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.71967676767676769</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.71954911433172308</v>
+      </c>
+      <c r="G13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.71967676767676769</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.71954911433172308</v>
-      </c>
-      <c r="G13" s="1">
-        <v>21.597750663757321</v>
-      </c>
-      <c r="H13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <v>0.71799999999999997</v>
@@ -3959,51 +3938,45 @@
       <c r="F14" s="1">
         <v>0.71788783942855072</v>
       </c>
-      <c r="G14" s="1">
-        <v>7.3510808944702148</v>
-      </c>
-      <c r="H14" s="1" t="b">
+      <c r="G14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.70965875947890344</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.70934672840327062</v>
+      </c>
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.71</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.70965875947890344</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.71</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.70934672840327062</v>
-      </c>
-      <c r="G15" s="1">
-        <v>23.60035943984985</v>
-      </c>
-      <c r="H15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
         <v>0.71</v>
@@ -4017,22 +3990,19 @@
       <c r="F16" s="1">
         <v>0.71023209283713484</v>
       </c>
-      <c r="G16" s="1">
-        <v>5.5891282558441162</v>
-      </c>
-      <c r="H16" s="1" t="b">
+      <c r="G16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>0.70099999999999996</v>
@@ -4046,22 +4016,19 @@
       <c r="F17" s="1">
         <v>0.70116154887885818</v>
       </c>
-      <c r="G17" s="1">
-        <v>39.111194610595703</v>
-      </c>
-      <c r="H17" s="1" t="b">
+      <c r="G17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C18" s="1">
         <v>0.68100000000000005</v>
@@ -4075,51 +4042,45 @@
       <c r="F18" s="1">
         <v>0.6811949419451887</v>
       </c>
-      <c r="G18" s="1">
-        <v>16.660394430160519</v>
-      </c>
-      <c r="H18" s="1" t="b">
+      <c r="G18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="H18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.6808912020762441</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.6809394687514746</v>
+      </c>
+      <c r="G19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.68100000000000005</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.6808912020762441</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.68100000000000005</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0.6809394687514746</v>
-      </c>
-      <c r="G19" s="1">
-        <v>11.840480327606199</v>
-      </c>
-      <c r="H19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1">
         <v>0.67900000000000005</v>
@@ -4133,22 +4094,19 @@
       <c r="F20" s="1">
         <v>0.67923508567341018</v>
       </c>
-      <c r="G20" s="1">
-        <v>35.40446400642395</v>
-      </c>
-      <c r="H20" s="1" t="b">
+      <c r="G20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1">
         <v>0.66400000000000003</v>
@@ -4162,51 +4120,45 @@
       <c r="F21" s="1">
         <v>0.6637081832218219</v>
       </c>
-      <c r="G21" s="1">
-        <v>21.695379018783569</v>
-      </c>
-      <c r="H21" s="1" t="b">
+      <c r="G21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="H21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.64801760051865098</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.647275450031503</v>
+      </c>
+      <c r="G22" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.64801760051865098</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.647275450031503</v>
-      </c>
-      <c r="G22" s="1">
-        <v>25.597458600997921</v>
-      </c>
-      <c r="H22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C23" s="1">
         <v>0.625</v>
@@ -4220,22 +4172,19 @@
       <c r="F23" s="1">
         <v>0.6235377939181922</v>
       </c>
-      <c r="G23" s="1">
-        <v>19.22005724906921</v>
-      </c>
-      <c r="H23" s="1" t="b">
+      <c r="G23" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1">
         <v>0.61699999999999999</v>
@@ -4249,51 +4198,45 @@
       <c r="F24" s="1">
         <v>0.61728049162902199</v>
       </c>
-      <c r="G24" s="1">
-        <v>4.6047906875610352</v>
-      </c>
-      <c r="H24" s="1" t="b">
+      <c r="G24" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="H24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.61098552766393432</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.61029536101683357</v>
+      </c>
+      <c r="G25" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.61</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.61098552766393432</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0.61</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0.61029536101683357</v>
-      </c>
-      <c r="G25" s="1">
-        <v>7.942906379699707</v>
-      </c>
-      <c r="H25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C26" s="1">
         <v>0.60899999999999999</v>
@@ -4307,22 +4250,19 @@
       <c r="F26" s="1">
         <v>0.60932071681026834</v>
       </c>
-      <c r="G26" s="1">
-        <v>22.450376510620121</v>
-      </c>
-      <c r="H26" s="1" t="b">
+      <c r="G26" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1">
         <v>0.60599999999999998</v>
@@ -4336,22 +4276,19 @@
       <c r="F27" s="1">
         <v>0.60634869909615519</v>
       </c>
-      <c r="G27" s="1">
-        <v>7.2929322719573966</v>
-      </c>
-      <c r="H27" s="1" t="b">
+      <c r="G27" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1">
         <v>0.60499999999999998</v>
@@ -4365,51 +4302,45 @@
       <c r="F28" s="1">
         <v>0.60514655218105695</v>
       </c>
-      <c r="G28" s="1">
-        <v>17.354134082794189</v>
-      </c>
-      <c r="H28" s="1" t="b">
+      <c r="G28" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="H28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.59531684174855992</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.59550588197428356</v>
+      </c>
+      <c r="G29" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0.59531684174855992</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="F29" s="1">
-        <v>0.59550588197428356</v>
-      </c>
-      <c r="G29" s="1">
-        <v>22.867355346679691</v>
-      </c>
-      <c r="H29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="1">
         <v>0.59099999999999997</v>
@@ -4423,22 +4354,19 @@
       <c r="F30" s="1">
         <v>0.59135831393456983</v>
       </c>
-      <c r="G30" s="1">
-        <v>21.181067228317261</v>
-      </c>
-      <c r="H30" s="1" t="b">
+      <c r="G30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1">
         <v>0.59</v>
@@ -4452,22 +4380,19 @@
       <c r="F31" s="1">
         <v>0.58964570898209334</v>
       </c>
-      <c r="G31" s="1">
-        <v>17.604587554931641</v>
-      </c>
-      <c r="H31" s="1" t="b">
+      <c r="G31" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="1">
         <v>0.57799999999999996</v>
@@ -4481,22 +4406,19 @@
       <c r="F32" s="1">
         <v>0.57756272229356953</v>
       </c>
-      <c r="G32" s="1">
-        <v>4.1407501697540283</v>
-      </c>
-      <c r="H32" s="1" t="b">
+      <c r="G32" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H32" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1">
         <v>0.55000000000000004</v>
@@ -4510,22 +4432,19 @@
       <c r="F33" s="1">
         <v>0.51141719216727521</v>
       </c>
-      <c r="G33" s="1">
-        <v>18.88773083686829</v>
-      </c>
-      <c r="H33" s="1" t="b">
+      <c r="G33" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" s="1">
         <v>0.53500000000000003</v>
@@ -4539,51 +4458,45 @@
       <c r="F34" s="1">
         <v>0.39628951352827552</v>
       </c>
-      <c r="G34" s="1">
-        <v>31.61168456077576</v>
-      </c>
-      <c r="H34" s="1" t="b">
+      <c r="G34" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.537320355392369</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.51526153049165468</v>
+      </c>
+      <c r="G35" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0.537320355392369</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0.51526153049165468</v>
-      </c>
-      <c r="G35" s="1">
-        <v>8.5970227718353271</v>
-      </c>
-      <c r="H35" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1">
         <v>0.50800000000000001</v>
@@ -4597,22 +4510,19 @@
       <c r="F36" s="1">
         <v>0.49214526854219948</v>
       </c>
-      <c r="G36" s="1">
-        <v>22.277244806289669</v>
-      </c>
-      <c r="H36" s="1" t="b">
+      <c r="G36" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="1">
         <v>0.505</v>
@@ -4626,25 +4536,646 @@
       <c r="F37" s="1">
         <v>0.5044429996749269</v>
       </c>
-      <c r="G37" s="1">
-        <v>4.5924437046051034</v>
-      </c>
-      <c r="H37" s="1" t="b">
+      <c r="G37" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>19</v>
+      <c r="H37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.66131698674395023</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.66112612328029441</v>
+      </c>
+      <c r="G38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.76872043682246882</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.76816364481636457</v>
+      </c>
+      <c r="G39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.66872063488253952</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.66729965496842469</v>
+      </c>
+      <c r="G40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.7201163853219833</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.7161181515617</v>
+      </c>
+      <c r="G41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.6551301595452339</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.65505918729953627</v>
+      </c>
+      <c r="G42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.752</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.75180193236714965</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.752</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.75182554517133948</v>
+      </c>
+      <c r="G43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.626</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.62672784931770142</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.626</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.62624136673200492</v>
+      </c>
+      <c r="G44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.67519781063952367</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.67427293011108036</v>
+      </c>
+      <c r="G45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.51014566922817761</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.45776748156722469</v>
+      </c>
+      <c r="G46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.78235963596359648</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.78119186002853502</v>
+      </c>
+      <c r="G47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.52607252772304636</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.52635359472902266</v>
+      </c>
+      <c r="G48" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.76313584277575064</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.76219925572526726</v>
+      </c>
+      <c r="G49" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.50259532054453182</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.47394856946557401</v>
+      </c>
+      <c r="G50" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.79563507156440805</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.7951386557779504</v>
+      </c>
+      <c r="G51" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.501</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.52047272727272731</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.501</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0.47520642428337528</v>
+      </c>
+      <c r="G52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.751</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.75077588466579304</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.751</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0.75071829038340665</v>
+      </c>
+      <c r="G53" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.8469572256750405</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0.84697096777108349</v>
+      </c>
+      <c r="G54" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.82593705293276121</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0.82595527279737802</v>
+      </c>
+      <c r="G55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.8161088382987598</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0.81604134565998965</v>
+      </c>
+      <c r="G56" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.77198915182642913</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0.77020624169348773</v>
+      </c>
+      <c r="G57" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.84120295554953739</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0.84072775479923767</v>
+      </c>
+      <c r="G58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.814189992067475</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0.81362235936769856</v>
+      </c>
+      <c r="G59" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.80602424242424242</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0.80568760064412226</v>
+      </c>
+      <c r="G60" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.77485764212582375</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0.77470371834607388</v>
+      </c>
+      <c r="G61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I37" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
+  <autoFilter ref="A1:H37" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="7">
       <filters>
         <filter val="cleaned"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H37">
     <sortCondition descending="1" ref="C2:C37"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4672,34 +5203,34 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.61699999999999999</v>
@@ -4713,7 +5244,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>0.505</v>
@@ -4727,7 +5258,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0.72899999999999998</v>
@@ -4741,7 +5272,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>0.57799999999999996</v>
@@ -4755,7 +5286,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0.71799999999999997</v>
@@ -4769,7 +5300,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0.71</v>
@@ -4783,7 +5314,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>3.8569999999999998</v>
@@ -4800,34 +5331,34 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
         <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26">
         <v>0.59099999999999997</v>
@@ -4841,7 +5372,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27">
         <v>0.55000000000000004</v>
@@ -4855,7 +5386,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28">
         <v>0.68100000000000005</v>
@@ -4869,7 +5400,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29">
         <v>0.59</v>
@@ -4883,7 +5414,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30">
         <v>0.66400000000000003</v>
@@ -4897,7 +5428,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31">
         <v>0.60499999999999998</v>
@@ -4911,7 +5442,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>3.681</v>
@@ -4927,4 +5458,643 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD02FC9-D4E6-48B2-BE65-58C03604CCD4}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="D1">
+        <v>0.66131698674395023</v>
+      </c>
+      <c r="E1">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="F1">
+        <v>0.66112612328029441</v>
+      </c>
+      <c r="G1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="D2">
+        <v>0.76872043682246882</v>
+      </c>
+      <c r="E2">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="F2">
+        <v>0.76816364481636457</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D3">
+        <v>0.66872063488253952</v>
+      </c>
+      <c r="E3">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="F3">
+        <v>0.66729965496842469</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.7201163853219833</v>
+      </c>
+      <c r="E4">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="F4">
+        <v>0.7161181515617</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="D5">
+        <v>0.6551301595452339</v>
+      </c>
+      <c r="E5">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F5">
+        <v>0.65505918729953627</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0.752</v>
+      </c>
+      <c r="D6">
+        <v>0.75180193236714965</v>
+      </c>
+      <c r="E6">
+        <v>0.752</v>
+      </c>
+      <c r="F6">
+        <v>0.75182554517133948</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0.626</v>
+      </c>
+      <c r="D7">
+        <v>0.62672784931770142</v>
+      </c>
+      <c r="E7">
+        <v>0.626</v>
+      </c>
+      <c r="F7">
+        <v>0.62624136673200492</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="D8">
+        <v>0.67519781063952367</v>
+      </c>
+      <c r="E8">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F8">
+        <v>0.67427293011108036</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.51014566922817761</v>
+      </c>
+      <c r="E9">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.45776748156722469</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="D10">
+        <v>0.78235963596359648</v>
+      </c>
+      <c r="E10">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="F10">
+        <v>0.78119186002853502</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="D11">
+        <v>0.52607252772304636</v>
+      </c>
+      <c r="E11">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="F11">
+        <v>0.52635359472902266</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.76313584277575064</v>
+      </c>
+      <c r="E12">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.76219925572526726</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0.49</v>
+      </c>
+      <c r="D13">
+        <v>0.50259532054453182</v>
+      </c>
+      <c r="E13">
+        <v>0.49</v>
+      </c>
+      <c r="F13">
+        <v>0.47394856946557401</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="D14">
+        <v>0.79563507156440805</v>
+      </c>
+      <c r="E14">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F14">
+        <v>0.7951386557779504</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>0.501</v>
+      </c>
+      <c r="D15">
+        <v>0.52047272727272731</v>
+      </c>
+      <c r="E15">
+        <v>0.501</v>
+      </c>
+      <c r="F15">
+        <v>0.47520642428337528</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>0.751</v>
+      </c>
+      <c r="D16">
+        <v>0.75077588466579304</v>
+      </c>
+      <c r="E16">
+        <v>0.751</v>
+      </c>
+      <c r="F16">
+        <v>0.75071829038340665</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="D17">
+        <v>0.8469572256750405</v>
+      </c>
+      <c r="E17">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="F17">
+        <v>0.84697096777108349</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="D18">
+        <v>0.82593705293276121</v>
+      </c>
+      <c r="E18">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="F18">
+        <v>0.82595527279737802</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="D19">
+        <v>0.8161088382987598</v>
+      </c>
+      <c r="E19">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F19">
+        <v>0.81604134565998965</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>0.77</v>
+      </c>
+      <c r="D20">
+        <v>0.77198915182642913</v>
+      </c>
+      <c r="E20">
+        <v>0.77</v>
+      </c>
+      <c r="F20">
+        <v>0.77020624169348773</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="D21">
+        <v>0.84120295554953739</v>
+      </c>
+      <c r="E21">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="F21">
+        <v>0.84072775479923767</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="D22">
+        <v>0.814189992067475</v>
+      </c>
+      <c r="E22">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="F22">
+        <v>0.81362235936769856</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="D23">
+        <v>0.80602424242424242</v>
+      </c>
+      <c r="E23">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="F23">
+        <v>0.80568760064412226</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D24">
+        <v>0.77485764212582375</v>
+      </c>
+      <c r="E24">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F24">
+        <v>0.77470371834607388</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>